<commit_message>
new notebook with a test of my best models
</commit_message>
<xml_diff>
--- a/docs/model_results_2best.xlsx
+++ b/docs/model_results_2best.xlsx
@@ -614,10 +614,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.68" customWidth="1"/>
-    <col min="2" max="2" width="27.44" customWidth="1"/>
-    <col min="3" max="3" width="43.88" customWidth="1"/>
-    <col min="4" max="4" width="27.91" customWidth="1"/>
+    <col min="1" max="1" width="39.85" customWidth="1"/>
+    <col min="2" max="2" width="43.53" customWidth="1"/>
+    <col min="3" max="3" width="66.23" customWidth="1"/>
+    <col min="4" max="4" width="45.59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>